<commit_message>
testes de mesa para o dia 22 ok
</commit_message>
<xml_diff>
--- a/Teste de mesa.xlsx
+++ b/Teste de mesa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaom\Desktop\Fatec\2°Semestre\Lp1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{144274D3-DB8B-4BE7-9D01-C1967C30C8EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12159D9D-06D4-4AFD-85F0-D22754F4B66C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6EBD7688-8B3F-4715-ADF4-E1A0B2A54EAC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
     <t>SAÍDA</t>
   </si>
   <si>
-    <t>TESTE DE MESA - EX 36</t>
+    <t>TESTE DE MESA - EX</t>
   </si>
 </sst>
 </file>
@@ -106,7 +106,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -136,19 +136,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -172,24 +159,30 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -507,23 +500,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57E4651C-EF3F-4CDE-BFD2-795D314AE26C}">
-  <dimension ref="D7:L12"/>
+  <dimension ref="D7:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:L9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="5" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="16.5703125" customWidth="1"/>
-    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="103.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="4:12" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="4:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D7" s="1" t="s">
         <v>1</v>
       </c>
@@ -532,70 +525,204 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-    </row>
-    <row r="8" spans="4:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D8" s="2"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3" t="s">
+    </row>
+    <row r="8" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="5"/>
-    </row>
-    <row r="10" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D10" s="6"/>
+    <row r="9" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D9" s="5"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D10" s="5"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-    </row>
-    <row r="11" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D11" s="6"/>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D11" s="5"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-    </row>
-    <row r="12" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
+      <c r="I11" s="3"/>
+    </row>
+    <row r="12" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D12" s="5"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D13" s="5"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D14" s="5"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D15" s="5"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D16" s="5"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="3"/>
+    </row>
+    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D17" s="5"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="3"/>
+    </row>
+    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D18" s="5"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="3"/>
+    </row>
+    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D19" s="5"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="3"/>
+    </row>
+    <row r="20" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D20" s="5"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+    </row>
+    <row r="21" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D21" s="5"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D22" s="5"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D23" s="5"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+    </row>
+    <row r="24" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D24" s="5"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+    </row>
+    <row r="25" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D25" s="5"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+    </row>
+    <row r="26" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D26" s="5"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+    </row>
+    <row r="27" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D27" s="5"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+    </row>
+    <row r="28" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D28" s="5"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+    </row>
+    <row r="29" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D29" s="5"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+    </row>
+    <row r="30" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D30" s="5"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+    </row>
+    <row r="31" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D31" s="7"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D7:L7"/>
+    <mergeCell ref="D7:I7"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
feat: exercícios - teste e codigo
</commit_message>
<xml_diff>
--- a/Teste de mesa.xlsx
+++ b/Teste de mesa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaom\Desktop\Fatec\2°Semestre\Lp1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12159D9D-06D4-4AFD-85F0-D22754F4B66C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2AB6D23-0C1D-412B-9AA8-1DE481F6E5E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6EBD7688-8B3F-4715-ADF4-E1A0B2A54EAC}"/>
   </bookViews>
@@ -161,9 +161,6 @@
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -183,6 +180,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -502,223 +502,222 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57E4651C-EF3F-4CDE-BFD2-795D314AE26C}">
   <dimension ref="D7:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScale="139" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="9.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="103.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="7" spans="4:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
     </row>
     <row r="8" spans="4:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4" t="s">
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D9" s="5"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="3"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="2"/>
     </row>
     <row r="10" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D10" s="5"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="3"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="2"/>
     </row>
     <row r="11" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D11" s="5"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="3"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="2"/>
     </row>
     <row r="12" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D12" s="5"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="3"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="2"/>
     </row>
     <row r="13" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D13" s="5"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="3"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="2"/>
     </row>
     <row r="14" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D14" s="5"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="3"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="2"/>
     </row>
     <row r="15" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D15" s="5"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="3"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="2"/>
     </row>
     <row r="16" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D16" s="5"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="3"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="2"/>
     </row>
     <row r="17" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D17" s="5"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="3"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="2"/>
     </row>
     <row r="18" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D18" s="5"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="3"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="2"/>
     </row>
     <row r="19" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D19" s="5"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="3"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="2"/>
     </row>
     <row r="20" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D20" s="5"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
     </row>
     <row r="21" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D21" s="5"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
     </row>
     <row r="22" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D22" s="5"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
     </row>
     <row r="23" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D23" s="5"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
     </row>
     <row r="24" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D24" s="5"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
     </row>
     <row r="25" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D25" s="5"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
     </row>
     <row r="26" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D26" s="5"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
     </row>
     <row r="27" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D27" s="5"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
     </row>
     <row r="28" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D28" s="5"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
     </row>
     <row r="29" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D29" s="5"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
     </row>
     <row r="30" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D30" s="5"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
     </row>
     <row r="31" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D31" s="7"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>